<commit_message>
Modified configuration of task types
Saved the task types in the sheet.
Created a named property to retrieve task types.
</commit_message>
<xml_diff>
--- a/template/Task_Tracker-Template.xlsx
+++ b/template/Task_Tracker-Template.xlsx
@@ -1,36 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\task_tracker\Project\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\task-tracker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687BD78C-68B8-4FC9-8D65-9CF56D9F0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Consolidated" sheetId="3" r:id="rId2"/>
     <sheet name="Hours" sheetId="2" r:id="rId3"/>
     <sheet name="Project-Task Mapping" sheetId="5" r:id="rId4"/>
+    <sheet name="TaskTypes" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="projectNames">OFFSET('Project-Task Mapping'!$A$1:$M$1, 0, 0, 1, COUNTA('Project-Task Mapping'!$A$1:$M$1))</definedName>
+    <definedName name="TaskTypes">OFFSET(TaskTypes!$A$2:$A$999, 0, 0, COUNTA(TaskTypes!$A$2:$A$999), 1)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -91,11 +103,14 @@
   <si>
     <t>TaskName</t>
   </si>
+  <si>
+    <t>TaskType</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -195,32 +210,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Task">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task">
       <calculatedColumnFormula>IF(B1="Break","Work","Break")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Project">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Project">
       <calculatedColumnFormula>IF(Table1[Task]="Break", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="TaskName">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TaskName">
       <calculatedColumnFormula>IF(Table1[Project]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Type">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Type">
       <calculatedColumnFormula>IF(Table1[TaskName]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Start" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNONTEXT(G1),IF(G1="","",G1),IF(Table10[Start]="","",Table10[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="End" dataDxfId="2"/>
-    <tableColumn id="5" name="Time Elapsed" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[End]="","",HOUR(Table1[End]-Table1[Start])*60 + MINUTE(Table1[End]-Table1[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Work Done">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Work Done">
       <calculatedColumnFormula>IF(Table1[Task]="Break","-")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -229,17 +244,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Work">
       <calculatedColumnFormula>SUMIF(Table1[Task], Table7[[#Headers],[Work]], Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Break">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Break">
       <calculatedColumnFormula>SUMIF(Table1[Task],Table7[[#Headers],[Break]],Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Ideal Work Hours"/>
-    <tableColumn id="4" name="Hours Remaining">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ideal Work Hours"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Hours Remaining">
       <calculatedColumnFormula>IF(Table8[Leaving Time]="","",TEXT(Table8[Leaving Time]-TIME(HOUR(NOW()),MINUTE(NOW()),0),"hh:mm"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -248,16 +263,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
-  <autoFilter ref="A5:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
+  <autoFilter ref="A5:C6" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Leaving Time" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="0">
       <calculatedColumnFormula>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Hours to Work">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Hours to Work">
       <calculatedColumnFormula>IF(Table7[Work]=0,"",Table7[Ideal Work Hours]-Table7[Work])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Break Time Remaining">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Break Time Remaining">
       <calculatedColumnFormula>IF(Table7[Break]=0,"",120-Table7[Break]*60)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -266,36 +281,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="E5:G6" totalsRowShown="0">
-  <autoFilter ref="E5:G6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table9" displayName="Table9" ref="E5:G6" totalsRowShown="0">
+  <autoFilter ref="E5:G6" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Lunch"/>
-    <tableColumn id="2" name="Prayer"/>
-    <tableColumn id="3" name="Morning"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Lunch"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Prayer"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Morning"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="F1:F2" totalsRowShown="0">
-  <autoFilter ref="F1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table10" displayName="Table10" ref="F1:F2" totalsRowShown="0">
+  <autoFilter ref="F1:F2" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Start"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Start"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Task">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Task">
       <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Hours">
-      <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Hours">
+      <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -564,31 +579,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,10 +632,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43862</v>
+        <v>44596</v>
       </c>
       <c r="B2" t="str">
         <f>IF(B1="Break","Work","Break")</f>
@@ -653,25 +668,28 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"-,B,BC,SL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>projectNames</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{6F82FE79-9F01-4C4E-AB63-9EC739B5A9C7}">
+      <formula1>TaskTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -705,7 +723,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>OFFSET('Project-Task Mapping'!$A$2:$J$8, 0, MATCH($C2, projectNames, 0)-1, 7, 1)</xm:f>
           </x14:formula1>
@@ -718,24 +736,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -752,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>SUMIF(Table1[Task], Table7[[#Headers],[Work]], Table1[Time Elapsed])/60</f>
         <v>0</v>
@@ -769,7 +787,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -789,7 +807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</f>
         <v/>
@@ -815,16 +833,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -832,93 +850,93 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</f>
         <v>-</v>
       </c>
       <c r="B2">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A2, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B3">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A3, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B4">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A4, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B5">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A5, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B6">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A6, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B7">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A7, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B8">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A8, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B9">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A9, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B10">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
@@ -931,39 +949,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D2" s="6"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O4" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>projectNames</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P4" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>OFFSET($A$2:$I$8, 0, MATCH($O2, projectNames, 0)-1, 7, 1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456B32DF-6822-4F5A-86A1-3877C97A967D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified configuration of task types (#6)
Saved the task types in the sheet.
Created a named property to retrieve task types.
</commit_message>
<xml_diff>
--- a/template/Task_Tracker-Template.xlsx
+++ b/template/Task_Tracker-Template.xlsx
@@ -1,36 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\task_tracker\Project\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\task-tracker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687BD78C-68B8-4FC9-8D65-9CF56D9F0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Consolidated" sheetId="3" r:id="rId2"/>
     <sheet name="Hours" sheetId="2" r:id="rId3"/>
     <sheet name="Project-Task Mapping" sheetId="5" r:id="rId4"/>
+    <sheet name="TaskTypes" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="projectNames">OFFSET('Project-Task Mapping'!$A$1:$M$1, 0, 0, 1, COUNTA('Project-Task Mapping'!$A$1:$M$1))</definedName>
+    <definedName name="TaskTypes">OFFSET(TaskTypes!$A$2:$A$999, 0, 0, COUNTA(TaskTypes!$A$2:$A$999), 1)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -91,11 +103,14 @@
   <si>
     <t>TaskName</t>
   </si>
+  <si>
+    <t>TaskType</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -195,32 +210,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Task">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task">
       <calculatedColumnFormula>IF(B1="Break","Work","Break")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Project">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Project">
       <calculatedColumnFormula>IF(Table1[Task]="Break", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="TaskName">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TaskName">
       <calculatedColumnFormula>IF(Table1[Project]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Type">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Type">
       <calculatedColumnFormula>IF(Table1[TaskName]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Start" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNONTEXT(G1),IF(G1="","",G1),IF(Table10[Start]="","",Table10[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="End" dataDxfId="2"/>
-    <tableColumn id="5" name="Time Elapsed" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[End]="","",HOUR(Table1[End]-Table1[Start])*60 + MINUTE(Table1[End]-Table1[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Work Done">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Work Done">
       <calculatedColumnFormula>IF(Table1[Task]="Break","-")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -229,17 +244,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table7" displayName="Table7" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Work">
       <calculatedColumnFormula>SUMIF(Table1[Task], Table7[[#Headers],[Work]], Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Break">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Break">
       <calculatedColumnFormula>SUMIF(Table1[Task],Table7[[#Headers],[Break]],Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Ideal Work Hours"/>
-    <tableColumn id="4" name="Hours Remaining">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ideal Work Hours"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Hours Remaining">
       <calculatedColumnFormula>IF(Table8[Leaving Time]="","",TEXT(Table8[Leaving Time]-TIME(HOUR(NOW()),MINUTE(NOW()),0),"hh:mm"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -248,16 +263,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
-  <autoFilter ref="A5:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
+  <autoFilter ref="A5:C6" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Leaving Time" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="0">
       <calculatedColumnFormula>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Hours to Work">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Hours to Work">
       <calculatedColumnFormula>IF(Table7[Work]=0,"",Table7[Ideal Work Hours]-Table7[Work])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Break Time Remaining">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Break Time Remaining">
       <calculatedColumnFormula>IF(Table7[Break]=0,"",120-Table7[Break]*60)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -266,36 +281,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="E5:G6" totalsRowShown="0">
-  <autoFilter ref="E5:G6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table9" displayName="Table9" ref="E5:G6" totalsRowShown="0">
+  <autoFilter ref="E5:G6" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Lunch"/>
-    <tableColumn id="2" name="Prayer"/>
-    <tableColumn id="3" name="Morning"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Lunch"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Prayer"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Morning"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="F1:F2" totalsRowShown="0">
-  <autoFilter ref="F1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table10" displayName="Table10" ref="F1:F2" totalsRowShown="0">
+  <autoFilter ref="F1:F2" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Start"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Start"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Task">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Task">
       <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Hours">
-      <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Hours">
+      <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -564,31 +579,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,10 +632,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43862</v>
+        <v>44596</v>
       </c>
       <c r="B2" t="str">
         <f>IF(B1="Break","Work","Break")</f>
@@ -653,25 +668,28 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H9" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"-,B,BC,SL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>projectNames</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{6F82FE79-9F01-4C4E-AB63-9EC739B5A9C7}">
+      <formula1>TaskTypes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -705,7 +723,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>OFFSET('Project-Task Mapping'!$A$2:$J$8, 0, MATCH($C2, projectNames, 0)-1, 7, 1)</xm:f>
           </x14:formula1>
@@ -718,24 +736,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -752,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>SUMIF(Table1[Task], Table7[[#Headers],[Work]], Table1[Time Elapsed])/60</f>
         <v>0</v>
@@ -769,7 +787,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -789,7 +807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="str">
         <f>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</f>
         <v/>
@@ -815,16 +833,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -832,93 +850,93 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</f>
         <v>-</v>
       </c>
       <c r="B2">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A2, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B3">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A3, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B4">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A4, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B5">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A5, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B6">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A6, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B7">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A7, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B8">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A8, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B9">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A9, Table1[TaskName]),), 0)), "")</f>
         <v/>
       </c>
       <c r="B10">
-        <f>SUMIF(Table1[TaskName],Table6[Task],Table1[Time Elapsed])/60</f>
+        <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
@@ -931,39 +949,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D2" s="6"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O4" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>projectNames</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P4" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>OFFSET($A$2:$I$8, 0, MATCH($O2, projectNames, 0)-1, 7, 1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456B32DF-6822-4F5A-86A1-3877C97A967D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Increased data range for project named value
</commit_message>
<xml_diff>
--- a/template/Task_Tracker-Template.xlsx
+++ b/template/Task_Tracker-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\task-tracker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687BD78C-68B8-4FC9-8D65-9CF56D9F0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36947B69-F7B7-4356-9FEB-C1F96AD3C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="TaskTypes" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="projectNames">OFFSET('Project-Task Mapping'!$A$1:$M$1, 0, 0, 1, COUNTA('Project-Task Mapping'!$A$1:$M$1))</definedName>
+    <definedName name="projectNames">OFFSET('Project-Task Mapping'!$A$1:$ALK$1, 0, 0, 1, COUNTA('Project-Task Mapping'!$A$1:$ALK$1))</definedName>
     <definedName name="TaskTypes">OFFSET(TaskTypes!$A$2:$A$999, 0, 0, COUNTA(TaskTypes!$A$2:$A$999), 1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -635,7 +635,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44596</v>
+        <v>44632</v>
       </c>
       <c r="B2" t="str">
         <f>IF(B1="Break","Work","Break")</f>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Template: Added project column in hours sheet
</commit_message>
<xml_diff>
--- a/template/Task_Tracker-Template.xlsx
+++ b/template/Task_Tracker-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\task-tracker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36947B69-F7B7-4356-9FEB-C1F96AD3C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1B90D6-2F92-4E10-9ECD-90AEBA1F753C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -168,7 +168,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.49803155613879818"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
@@ -184,18 +199,6 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -213,7 +216,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
   <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="6">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task">
@@ -228,11 +231,11 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Type">
       <calculatedColumnFormula>IF(Table1[TaskName]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="5">
       <calculatedColumnFormula>IF(ISNONTEXT(G1),IF(G1="","",G1),IF(Table10[Start]="","",Table10[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[End]="","",HOUR(Table1[End]-Table1[Start])*60 + MINUTE(Table1[End]-Table1[Start]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Work Done">
@@ -266,7 +269,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
   <autoFilter ref="A5:C6" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="2">
       <calculatedColumnFormula>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Hours to Work">
@@ -303,11 +306,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="3" xr3:uid="{2CD0955F-6A21-4DBE-B954-757389A53982}" name="Project" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Task">
-      <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Hours">
       <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</calculatedColumnFormula>
@@ -635,7 +641,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44632</v>
+        <v>44677</v>
       </c>
       <c r="B2" t="str">
         <f>IF(B1="Break","Work","Break")</f>
@@ -834,110 +840,161 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</f>
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
         <v>-</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B1, Table1[TaskName]),), 0)), "")</f>
+        <v>-</v>
+      </c>
+      <c r="C2">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A2, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B3">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B2, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C3">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A3, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B4">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B3, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C4">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A4, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B5">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B4, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C5">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A5, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B6">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B5, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C6">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A6, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B7">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B6, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C7">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A7, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B8">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B7, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C8">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A8, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B9">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B8, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C9">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A9, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B10">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B9, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C10">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15" t="str">
+        <f>INDEX(Table1[Project], MATCH(B2, Table1[TaskName], 0))</f>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Template: Added project column in hours sheet (#24)
</commit_message>
<xml_diff>
--- a/template/Task_Tracker-Template.xlsx
+++ b/template/Task_Tracker-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Personal\task-tracker\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36947B69-F7B7-4356-9FEB-C1F96AD3C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1B90D6-2F92-4E10-9ECD-90AEBA1F753C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -168,7 +168,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="90">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="0" tint="-0.49803155613879818"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
@@ -184,18 +199,6 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="90">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color theme="0" tint="-0.49803155613879818"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -213,7 +216,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0">
   <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="6">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task">
@@ -228,11 +231,11 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Type">
       <calculatedColumnFormula>IF(Table1[TaskName]="-", "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Start" dataDxfId="5">
       <calculatedColumnFormula>IF(ISNONTEXT(G1),IF(G1="","",G1),IF(Table10[Start]="","",Table10[Start]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="End" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Time Elapsed" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[End]="","",HOUR(Table1[End]-Table1[Start])*60 + MINUTE(Table1[End]-Table1[Start]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Work Done">
@@ -266,7 +269,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A5:C6" totalsRowShown="0">
   <autoFilter ref="A5:C6" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Leaving Time" dataDxfId="2">
       <calculatedColumnFormula>IF(Table10[Start]="","",Table10[Start]+TIME(8,50,0))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Hours to Work">
@@ -303,11 +306,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table6" displayName="Table6" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="3" xr3:uid="{2CD0955F-6A21-4DBE-B954-757389A53982}" name="Project" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Task">
-      <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B1, Table1[TaskName]),), 0)), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Hours">
       <calculatedColumnFormula>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</calculatedColumnFormula>
@@ -635,7 +641,7 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44632</v>
+        <v>44677</v>
       </c>
       <c r="B2" t="str">
         <f>IF(B1="Break","Work","Break")</f>
@@ -834,110 +840,161 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A1, Table1[TaskName]),), 0)), "")</f>
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
         <v>-</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B1, Table1[TaskName]),), 0)), "")</f>
+        <v>-</v>
+      </c>
+      <c r="C2">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A2, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B3">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B2, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C3">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A3, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B4">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B3, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C4">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A4, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B5">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B4, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C5">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A5, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B6">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B5, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C6">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A6, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B7">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B6, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C7">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A7, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B8">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B7, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C8">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A8, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B9">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B8, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C9">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($A$1:$A9, Table1[TaskName]),), 0)), "")</f>
-        <v/>
-      </c>
-      <c r="B10">
+        <f>IFERROR(INDEX(Table1[Project], MATCH(Table6[[#This Row],[Task]], Table1[TaskName], 0)), "")</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IFERROR(INDEX(Table1[TaskName], MATCH(0, INDEX(COUNTIF($B$1:$B9, Table1[TaskName]),), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="C10">
         <f>SUMIF(Table1[TaskName],Table6[[#This Row],[Task]],Table1[Time Elapsed])/60</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15" t="str">
+        <f>INDEX(Table1[Project], MATCH(B2, Table1[TaskName], 0))</f>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>